<commit_message>
update analyses world cafe
</commit_message>
<xml_diff>
--- a/Analyses/world cafe/outputs/openQuestions.xlsx
+++ b/Analyses/world cafe/outputs/openQuestions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -95,13 +95,42 @@
     <t>13</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
+    <t>Can survive damage, might be able to reach places/be used at places, where softness is a big advantage.</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>sensitive objects (medical) , 
+harsh environments (marine)</t>
+  </si>
+  <si>
     <t>They can be more adaptive, shape-change, and responsive.</t>
+  </si>
+  <si>
+    <t>Human machine Interaction
+Fitting through tight spaces</t>
   </si>
   <si>
     <t>large elastic deformation of the robot: in tight spaces, interaction with fragile objects</t>
@@ -139,6 +168,22 @@
     <t>Can be put in different spaces where the robots with hard counterparts are not accessible</t>
   </si>
   <si>
+    <t>Not within my field of expertise.</t>
+  </si>
+  <si>
+    <t>Medicine, care</t>
+  </si>
+  <si>
+    <t>Interaction of soft robots with humans might be safer due to usage of less stiff material.</t>
+  </si>
+  <si>
+    <t>Replacing real parts</t>
+  </si>
+  <si>
+    <t>different, additional fields of applications. 
+Long-lasting</t>
+  </si>
+  <si>
     <t>can adapt to different situations/conditions
 can handle physical damage better</t>
   </si>
@@ -150,6 +195,10 @@
 More interesting </t>
   </si>
   <si>
+    <t>Less likely to hurt people
+Fitting through tight spaces</t>
+  </si>
+  <si>
     <t>less risk for injury when interacting with the living world</t>
   </si>
   <si>
@@ -179,6 +228,13 @@
     <t>they are flexible and light</t>
   </si>
   <si>
+    <t>More flexible usage and less energy and ressource costly.</t>
+  </si>
+  <si>
+    <t>nicer feeling when touched
+more adaptive to human skin</t>
+  </si>
+  <si>
     <t>slow response, limited functionality</t>
   </si>
   <si>
@@ -198,6 +254,12 @@
     <t>hard to incorporate multiple functions and implement robustness</t>
   </si>
   <si>
+    <t>More flexible structure could give them a more naturalm shape.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy-and resource saving </t>
+  </si>
+  <si>
     <t xml:space="preserve">Less dangerous for people. </t>
   </si>
   <si>
@@ -213,6 +275,9 @@
     <t>More life-like means they could be easier to be accepted or seen for everyday's tasks</t>
   </si>
   <si>
+    <t>Higher acceptance and they might seem to be easier understood.</t>
+  </si>
+  <si>
     <t>More interaction with humans:)</t>
   </si>
   <si>
@@ -220,6 +285,15 @@
   </si>
   <si>
     <t>They should not become too human-like</t>
+  </si>
+  <si>
+    <t>More light-weight material could lower energy consumption during life span.</t>
+  </si>
+  <si>
+    <t>Its soft therefore, life-like.</t>
+  </si>
+  <si>
+    <t>at the moment soft robots consist of many different elements, which needs to be manufactured in complex processes. This is also problematic for recycling.</t>
   </si>
   <si>
     <t>can handly physical damag better -&gt; longer lasting</t>
@@ -236,6 +310,12 @@
   </si>
   <si>
     <t>Soft robots have the potential to be more sustainable than rigid robots because of no/reduced need for electronics and rare earths. Currently however, the possibilities such as biodegradable plastics beeing used and using green energy to generate pneumatic/hydraulic energy are inferior to simply sticking an electrically powered pneumatic pump somewhere in the circuit, which is far less efficient than simply using the electric energy to drive motors and such in the first place.</t>
+  </si>
+  <si>
+    <t>Some questions were repeating</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>Sometimes I found it difficult to answer some questions. That could be because the questions werenot self-explainatory enough, or I'm just not used to these type of studies/questions and therefore struggled a bit</t>
@@ -357,43 +437,43 @@
         <v>1.0</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="O2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -404,43 +484,43 @@
         <v>3.0</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
@@ -451,43 +531,43 @@
         <v>4.0</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="O4" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
@@ -498,43 +578,43 @@
         <v>5.0</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
@@ -542,46 +622,46 @@
         <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>16.0</v>
+        <v>7.0</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="L6" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="M6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="O6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -589,46 +669,46 @@
         <v>19</v>
       </c>
       <c r="B7" t="n">
-        <v>18.0</v>
+        <v>8.0</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="N7" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="O7" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
@@ -636,46 +716,46 @@
         <v>20</v>
       </c>
       <c r="B8" t="n">
-        <v>19.0</v>
+        <v>9.0</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -683,46 +763,46 @@
         <v>21</v>
       </c>
       <c r="B9" t="n">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
@@ -733,43 +813,43 @@
         <v>21.0</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="M10" t="s">
         <v>14</v>
       </c>
       <c r="N10" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -777,46 +857,46 @@
         <v>23</v>
       </c>
       <c r="B11" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O11" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
@@ -824,10 +904,10 @@
         <v>24</v>
       </c>
       <c r="B12" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
@@ -836,34 +916,34 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
       </c>
       <c r="J12" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="L12" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="M12" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="N12" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="O12" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -871,46 +951,46 @@
         <v>25</v>
       </c>
       <c r="B13" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="K13" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="N13" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="O13" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -918,46 +998,328 @@
         <v>26</v>
       </c>
       <c r="B14" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="I14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="J14" t="s">
+      <c r="B15" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="K14" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" t="s">
-        <v>74</v>
+      <c r="B16" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
+        <v>83</v>
+      </c>
+      <c r="M17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N18" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>